<commit_message>
import export and getPoints all work
</commit_message>
<xml_diff>
--- a/data-files/OutExcel2.xlsx
+++ b/data-files/OutExcel2.xlsx
@@ -5,9 +5,10 @@
   <sheets>
     <sheet name="Defs" sheetId="1" r:id="rId1"/>
     <sheet name="Point Defs" sheetId="2" r:id="rId2"/>
-    <sheet name="Entries Base" sheetId="3" r:id="rId3"/>
+    <sheet name="Entry Base" sheetId="3" r:id="rId3"/>
     <sheet name="Entry Points" sheetId="4" r:id="rId4"/>
-    <sheet name="Tags" sheetId="5" r:id="rId5"/>
+    <sheet name="Tag Defs" sheetId="5" r:id="rId5"/>
+    <sheet name="Tags" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -437,57 +438,57 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lglrnj0x.0qa55</v>
+        <v>lgr0q1t4-3lil</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-17T23:30:00.476</v>
+        <v>2023-04-21T15:42:45.553</v>
       </c>
       <c r="C2" t="str">
-        <v>2023-04-17T23:30:00.476</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
+        <v>lgr0q1te</v>
+      </c>
+      <c r="D2" t="str">
+        <v>FALSE</v>
       </c>
       <c r="E2" t="str">
-        <v>0plpu</v>
+        <v>05a8</v>
       </c>
       <c r="F2" t="str">
-        <v>twooo</v>
+        <v>afree</v>
       </c>
       <c r="G2" t="str">
-        <v>2️⃣</v>
+        <v>3️⃣</v>
       </c>
       <c r="H2" t="str">
-        <v>now with a description</v>
+        <v>Edited with description!</v>
       </c>
       <c r="I2" t="str">
-        <v>WEEK</v>
+        <v>SECOND</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lglrnj19.52rnu</v>
+        <v>lgr0q1te-5odh</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-17T23:30:00.477</v>
+        <v>2023-04-21T15:42:45.554</v>
       </c>
       <c r="C3" t="str">
-        <v>2023-04-17T23:30:00.477</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
+        <v>lgr0q1te</v>
+      </c>
+      <c r="D3" t="str">
+        <v>FALSE</v>
       </c>
       <c r="E3" t="str">
-        <v>490hh</v>
+        <v>7gor</v>
       </c>
       <c r="F3" t="str">
-        <v>four</v>
+        <v>Five</v>
       </c>
       <c r="G3" t="str">
-        <v>🕒</v>
+        <v>5️⃣</v>
       </c>
       <c r="H3" t="str">
-        <v>Set a description</v>
+        <v>not in first file, added to second</v>
       </c>
       <c r="I3" t="str">
         <v>SECOND</v>
@@ -502,7 +503,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -545,16 +546,54 @@
         <v>_format</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>lgr0q1te-9rqg</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2023-04-21T15:42:45.555</v>
+      </c>
+      <c r="C2" t="str">
+        <v>lgr0q1tf</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <v>e0bq</v>
+      </c>
+      <c r="F2" t="str">
+        <v>0pc6</v>
+      </c>
+      <c r="G2" t="str">
+        <v>updated label</v>
+      </c>
+      <c r="H2" t="str">
+        <v>☝️</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Set a description</v>
+      </c>
+      <c r="J2" t="str">
+        <v>BOOL</v>
+      </c>
+      <c r="K2" t="str">
+        <v>COUNT</v>
+      </c>
+      <c r="L2" t="str">
+        <v>TEXT</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -576,17 +615,103 @@
         <v>_did</v>
       </c>
       <c r="F1" t="str">
+        <v>_eid</v>
+      </c>
+      <c r="G1" t="str">
+        <v>_period</v>
+      </c>
+      <c r="H1" t="str">
         <v>_note</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>_uid</v>
+      </c>
+      <c r="B1" t="str">
+        <v>_created</v>
+      </c>
+      <c r="C1" t="str">
+        <v>_updated</v>
+      </c>
+      <c r="D1" t="str">
+        <v>_deleted</v>
+      </c>
+      <c r="E1" t="str">
+        <v>_did</v>
+      </c>
+      <c r="F1" t="str">
+        <v>_pid</v>
+      </c>
+      <c r="G1" t="str">
+        <v>_eid</v>
+      </c>
+      <c r="H1" t="str">
+        <v>_val</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>_uid</v>
+      </c>
+      <c r="B1" t="str">
+        <v>_created</v>
+      </c>
+      <c r="C1" t="str">
+        <v>_updated</v>
+      </c>
+      <c r="D1" t="str">
+        <v>_deleted</v>
+      </c>
+      <c r="E1" t="str">
+        <v>_tid</v>
+      </c>
+      <c r="F1" t="str">
+        <v>_lbl</v>
+      </c>
+      <c r="G1" t="str">
+        <v>_emoji</v>
+      </c>
+      <c r="H1" t="str">
+        <v>_desc</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -613,7 +738,7 @@
         <v>_pid</v>
       </c>
       <c r="G1" t="str">
-        <v>_val</v>
+        <v>tid</v>
       </c>
     </row>
   </sheetData>
@@ -621,38 +746,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:G1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>_uid</v>
-      </c>
-      <c r="B1" t="str">
-        <v>_created</v>
-      </c>
-      <c r="C1" t="str">
-        <v>_updated</v>
-      </c>
-      <c r="D1" t="str">
-        <v>_deleted</v>
-      </c>
-      <c r="E1" t="str">
-        <v>_tid</v>
-      </c>
-      <c r="F1" t="str">
-        <v>_lbl</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F1"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>